<commit_message>
WPFDragDrop - fix design of UI items to be close to picture.
</commit_message>
<xml_diff>
--- a/WPFDragDrop/Description/task.xlsx
+++ b/WPFDragDrop/Description/task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\P\S0GITHUB\J-2020-Demos\WPFDragDrop\Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D61A849-4F94-49B3-961A-805906F6D737}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF08334-E522-4551-B53D-4B18DBEF3FB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31650" yWindow="435" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Create a WPF desktop application displaying list of draggable items</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>just design</t>
+  </si>
+  <si>
+    <t>most</t>
   </si>
 </sst>
 </file>
@@ -475,15 +481,24 @@
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="52.5" x14ac:dyDescent="0.4">
       <c r="B7" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
WPFDragDrop - drag and drop tested, at least works for acceptance and some data copy, showling list of dropped.
</commit_message>
<xml_diff>
--- a/WPFDragDrop/Description/task.xlsx
+++ b/WPFDragDrop/Description/task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\P\S0GITHUB\J-2020-Demos\WPFDragDrop\Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF08334-E522-4551-B53D-4B18DBEF3FB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231AAC3B-658D-436B-8C5F-D7835385312F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31650" yWindow="435" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Create a WPF desktop application displaying list of draggable items</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>most</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
@@ -445,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -505,11 +508,17 @@
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="52.5" x14ac:dyDescent="0.4">
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
@@ -520,25 +529,40 @@
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="52.5" x14ac:dyDescent="0.4">
       <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B15" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="52.5" x14ac:dyDescent="0.4">
       <c r="B16" s="3" t="s">
         <v>21</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
WPFDragDrop - fixed recording of dragged / dropped item.
</commit_message>
<xml_diff>
--- a/WPFDragDrop/Description/task.xlsx
+++ b/WPFDragDrop/Description/task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\P\S0GITHUB\J-2020-Demos\WPFDragDrop\Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231AAC3B-658D-436B-8C5F-D7835385312F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DC5262-58BA-4D22-9A70-F175E45A55B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31650" yWindow="435" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Create a WPF desktop application displaying list of draggable items</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>Not now</t>
+  </si>
+  <si>
+    <t>Works Unique, does not duplicate</t>
   </si>
 </sst>
 </file>
@@ -448,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -565,42 +574,57 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="52.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="52.5" x14ac:dyDescent="0.4">
       <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="78.75" x14ac:dyDescent="0.4">
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="105" x14ac:dyDescent="0.4">
       <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="52.5" x14ac:dyDescent="0.4">
+      <c r="C20" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="52.5" x14ac:dyDescent="0.4">
       <c r="B21" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="52.5" x14ac:dyDescent="0.4">
+      <c r="C21" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="52.5" x14ac:dyDescent="0.4">
       <c r="B22" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="52.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="52.5" x14ac:dyDescent="0.4">
       <c r="B25" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C25" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
WPFDragDrop - reset button (can not show) and programmed.
</commit_message>
<xml_diff>
--- a/WPFDragDrop/Description/task.xlsx
+++ b/WPFDragDrop/Description/task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\P\S0GITHUB\J-2020-Demos\WPFDragDrop\Description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DC5262-58BA-4D22-9A70-F175E45A55B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C8FFB7-9E6F-4419-B675-8F317B52C3AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31650" yWindow="435" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Create a WPF desktop application displaying list of draggable items</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Works Unique, does not duplicate</t>
+  </si>
+  <si>
+    <t>Just programmed it.</t>
   </si>
 </sst>
 </file>
@@ -458,7 +461,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -628,6 +631,9 @@
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C27" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>